<commit_message>
began working on rotowire
</commit_message>
<xml_diff>
--- a/Daniel/Table_column_names.xlsx
+++ b/Daniel/Table_column_names.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chand\Documents\GitHub\NFL-ETL-Project\Daniel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CEF5F9A-1CAD-4699-900B-C7E559B34E98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7786865A-8457-45C7-81B2-BD19CF024291}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{0033C061-D952-47A4-8EB3-0997677FD57E}"/>
+    <workbookView xWindow="2370" yWindow="2370" windowWidth="14400" windowHeight="7380" activeTab="2" xr2:uid="{0033C061-D952-47A4-8EB3-0997677FD57E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Stats" sheetId="1" r:id="rId1"/>
+    <sheet name="Roster" sheetId="2" r:id="rId2"/>
+    <sheet name="Fantasy" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="127">
   <si>
     <t>Name</t>
   </si>
@@ -299,9 +301,6 @@
     <t>('Tackles', 'SOLO')</t>
   </si>
   <si>
-    <t>roster</t>
-  </si>
-  <si>
     <t>Special</t>
   </si>
   <si>
@@ -324,6 +323,99 @@
   </si>
   <si>
     <t>College</t>
+  </si>
+  <si>
+    <t>te</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>TGT</t>
+  </si>
+  <si>
+    <t>Y/R</t>
+  </si>
+  <si>
+    <t>LG</t>
+  </si>
+  <si>
+    <t>20+</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>FPTS</t>
+  </si>
+  <si>
+    <t>FPTS/G</t>
+  </si>
+  <si>
+    <t>OWN</t>
+  </si>
+  <si>
+    <t>wr</t>
+  </si>
+  <si>
+    <t>lb</t>
+  </si>
+  <si>
+    <t>TACKLE</t>
+  </si>
+  <si>
+    <t>ASSIST</t>
+  </si>
+  <si>
+    <t>PD</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>DEF TD</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>qb</t>
+  </si>
+  <si>
+    <t>SACKS</t>
+  </si>
+  <si>
+    <t>Y/A</t>
+  </si>
+  <si>
+    <t>PCT</t>
+  </si>
+  <si>
+    <t>rb</t>
+  </si>
+  <si>
+    <t>dst</t>
+  </si>
+  <si>
+    <t>SFTY</t>
+  </si>
+  <si>
+    <t>SPC TD</t>
+  </si>
+  <si>
+    <t>dl</t>
+  </si>
+  <si>
+    <t>db</t>
   </si>
 </sst>
 </file>
@@ -675,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37663115-D1F9-4988-8F14-6F8CFE8E8A8E}">
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1193,102 +1285,582 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.75">
-      <c r="A20" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{363CFBB8-54BA-4250-B205-9512BBE76B5B}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.75">
-      <c r="A21" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.75">
-      <c r="B22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D6" t="s">
         <v>91</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E6" t="s">
         <v>92</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F6" t="s">
         <v>93</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G6" t="s">
         <v>94</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H6" t="s">
         <v>95</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF75C0B5-B193-433F-A4D3-7931E048C022}">
+  <dimension ref="A1:T16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
         <v>96</v>
       </c>
-      <c r="I22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.75">
-      <c r="A23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.75">
-      <c r="B24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" t="s">
-        <v>91</v>
-      </c>
-      <c r="D24" t="s">
-        <v>92</v>
-      </c>
-      <c r="E24" t="s">
-        <v>93</v>
-      </c>
-      <c r="F24" t="s">
-        <v>94</v>
-      </c>
-      <c r="G24" t="s">
-        <v>95</v>
-      </c>
-      <c r="H24" t="s">
-        <v>96</v>
-      </c>
-      <c r="I24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.75">
-      <c r="A25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.75">
-      <c r="B26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" t="s">
-        <v>91</v>
-      </c>
-      <c r="D26" t="s">
-        <v>92</v>
-      </c>
-      <c r="E26" t="s">
-        <v>93</v>
-      </c>
-      <c r="F26" t="s">
-        <v>94</v>
-      </c>
-      <c r="G26" t="s">
-        <v>95</v>
-      </c>
-      <c r="H26" t="s">
-        <v>96</v>
-      </c>
-      <c r="I26" t="s">
-        <v>15</v>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" t="s">
+        <v>103</v>
+      </c>
+      <c r="O2" t="s">
+        <v>104</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>106</v>
+      </c>
+      <c r="R2" t="s">
+        <v>107</v>
+      </c>
+      <c r="S2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I4" t="s">
+        <v>102</v>
+      </c>
+      <c r="J4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" t="s">
+        <v>103</v>
+      </c>
+      <c r="O4" t="s">
+        <v>104</v>
+      </c>
+      <c r="P4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>106</v>
+      </c>
+      <c r="R4" t="s">
+        <v>107</v>
+      </c>
+      <c r="S4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="B6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" t="s">
+        <v>113</v>
+      </c>
+      <c r="J6" t="s">
+        <v>114</v>
+      </c>
+      <c r="K6" t="s">
+        <v>115</v>
+      </c>
+      <c r="L6" t="s">
+        <v>104</v>
+      </c>
+      <c r="M6" t="s">
+        <v>105</v>
+      </c>
+      <c r="N6" t="s">
+        <v>106</v>
+      </c>
+      <c r="O6" t="s">
+        <v>107</v>
+      </c>
+      <c r="P6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="B8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" t="s">
+        <v>119</v>
+      </c>
+      <c r="I8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K8" t="s">
+        <v>118</v>
+      </c>
+      <c r="L8" t="s">
+        <v>54</v>
+      </c>
+      <c r="M8" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" t="s">
+        <v>45</v>
+      </c>
+      <c r="O8" t="s">
+        <v>103</v>
+      </c>
+      <c r="P8" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>105</v>
+      </c>
+      <c r="R8" t="s">
+        <v>106</v>
+      </c>
+      <c r="S8" t="s">
+        <v>107</v>
+      </c>
+      <c r="T8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="B10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>119</v>
+      </c>
+      <c r="G10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" t="s">
+        <v>99</v>
+      </c>
+      <c r="L10" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10" t="s">
+        <v>100</v>
+      </c>
+      <c r="N10" t="s">
+        <v>45</v>
+      </c>
+      <c r="O10" t="s">
+        <v>103</v>
+      </c>
+      <c r="P10" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>105</v>
+      </c>
+      <c r="R10" t="s">
+        <v>106</v>
+      </c>
+      <c r="S10" t="s">
+        <v>107</v>
+      </c>
+      <c r="T10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="B12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G12" t="s">
+        <v>113</v>
+      </c>
+      <c r="H12" t="s">
+        <v>115</v>
+      </c>
+      <c r="I12" t="s">
+        <v>123</v>
+      </c>
+      <c r="J12" t="s">
+        <v>124</v>
+      </c>
+      <c r="K12" t="s">
+        <v>104</v>
+      </c>
+      <c r="L12" t="s">
+        <v>105</v>
+      </c>
+      <c r="M12" t="s">
+        <v>106</v>
+      </c>
+      <c r="N12" t="s">
+        <v>107</v>
+      </c>
+      <c r="O12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="B14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" t="s">
+        <v>111</v>
+      </c>
+      <c r="F14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" t="s">
+        <v>112</v>
+      </c>
+      <c r="H14" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" t="s">
+        <v>113</v>
+      </c>
+      <c r="J14" t="s">
+        <v>114</v>
+      </c>
+      <c r="K14" t="s">
+        <v>115</v>
+      </c>
+      <c r="L14" t="s">
+        <v>104</v>
+      </c>
+      <c r="M14" t="s">
+        <v>105</v>
+      </c>
+      <c r="N14" t="s">
+        <v>106</v>
+      </c>
+      <c r="O14" t="s">
+        <v>107</v>
+      </c>
+      <c r="P14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="B16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" t="s">
+        <v>112</v>
+      </c>
+      <c r="H16" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" t="s">
+        <v>113</v>
+      </c>
+      <c r="J16" t="s">
+        <v>114</v>
+      </c>
+      <c r="K16" t="s">
+        <v>115</v>
+      </c>
+      <c r="L16" t="s">
+        <v>104</v>
+      </c>
+      <c r="M16" t="s">
+        <v>105</v>
+      </c>
+      <c r="N16" t="s">
+        <v>106</v>
+      </c>
+      <c r="O16" t="s">
+        <v>107</v>
+      </c>
+      <c r="P16" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>